<commit_message>
update manual test case
</commit_message>
<xml_diff>
--- a/test_case_katalon.xlsx
+++ b/test_case_katalon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dangh\Desktop\Amaris_QA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{711BF7FE-B095-4D16-845F-D7340CDE783D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37457A81-D9E4-49DB-83F1-6162E5E41C03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29760" yWindow="-3795" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="165">
   <si>
     <t>TEST CASE TEMPLATE</t>
   </si>
@@ -535,6 +535,26 @@
   <si>
     <t xml:space="preserve">Coupon "aaaa" does not exist!
 </t>
+  </si>
+  <si>
+    <t>TC020</t>
+  </si>
+  <si>
+    <t>Register_Select payment with out input info</t>
+  </si>
+  <si>
+    <t>2. leave all input block blank</t>
+  </si>
+  <si>
+    <t>3. click "continue to payment"</t>
+  </si>
+  <si>
+    <t>Billing First Name is a required field.
+Billing Last Name is a required field.
+Billing Phone is a required field.
+Billing Address is a required field.
+Billing Town / City is a required field.
+Billing Postcode / ZIP is a required field.</t>
   </si>
 </sst>
 </file>
@@ -1178,8 +1198,8 @@
   </sheetPr>
   <dimension ref="A1:AD1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" topLeftCell="E76" workbookViewId="0">
+      <selection activeCell="J81" sqref="J81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
@@ -4275,12 +4295,20 @@
       <c r="AC78" s="5"/>
       <c r="AD78" s="5"/>
     </row>
-    <row r="79" spans="1:30" ht="17.399999999999999">
+    <row r="79" spans="1:30" ht="30">
       <c r="A79" s="6"/>
-      <c r="B79" s="22"/>
-      <c r="C79" s="22"/>
-      <c r="D79" s="21"/>
-      <c r="E79" s="21"/>
+      <c r="B79" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="C79" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E79" s="21" t="s">
+        <v>98</v>
+      </c>
       <c r="F79" s="22"/>
       <c r="G79" s="22"/>
       <c r="H79" s="22"/>
@@ -4307,17 +4335,27 @@
       <c r="AC79" s="5"/>
       <c r="AD79" s="5"/>
     </row>
-    <row r="80" spans="1:30" ht="17.399999999999999">
+    <row r="80" spans="1:30" ht="195">
       <c r="A80" s="6"/>
       <c r="B80" s="22"/>
       <c r="C80" s="22"/>
       <c r="D80" s="21"/>
-      <c r="E80" s="21"/>
+      <c r="E80" s="21" t="s">
+        <v>162</v>
+      </c>
       <c r="F80" s="22"/>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="22"/>
-      <c r="J80" s="22"/>
+      <c r="G80" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="H80" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="I80" s="36" t="s">
+        <v>154</v>
+      </c>
+      <c r="J80" s="22" t="s">
+        <v>21</v>
+      </c>
       <c r="K80" s="25"/>
       <c r="L80" s="25"/>
       <c r="M80" s="22"/>
@@ -4339,12 +4377,14 @@
       <c r="AC80" s="5"/>
       <c r="AD80" s="5"/>
     </row>
-    <row r="81" spans="1:30" ht="17.399999999999999">
+    <row r="81" spans="1:30" ht="26.4">
       <c r="A81" s="6"/>
       <c r="B81" s="22"/>
       <c r="C81" s="26"/>
       <c r="D81" s="21"/>
-      <c r="E81" s="21"/>
+      <c r="E81" s="21" t="s">
+        <v>163</v>
+      </c>
       <c r="F81" s="22"/>
       <c r="G81" s="22"/>
       <c r="H81" s="22"/>
@@ -34014,6 +34054,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>